<commit_message>
[ FIX SIGNAL ATTRIBUTE GREP FAIL ]
</commit_message>
<xml_diff>
--- a/dbc/ALIEN_OF_DBC/ARS408_can_database_ch01.xlsx
+++ b/dbc/ALIEN_OF_DBC/ARS408_can_database_ch01.xlsx
@@ -3020,7 +3020,7 @@
         <v>43</v>
       </c>
       <c r="Z13" s="3">
-        <v>-2.5</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="3" t="s">
         <v>43</v>
@@ -3282,7 +3282,7 @@
         <v>43</v>
       </c>
       <c r="Z15" s="3">
-        <v>-180</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="3" t="s">
         <v>43</v>
@@ -3675,7 +3675,7 @@
         <v>43</v>
       </c>
       <c r="Z18" s="3">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="3" t="s">
         <v>43</v>
@@ -4199,7 +4199,7 @@
         <v>43</v>
       </c>
       <c r="Z22" s="3">
-        <v>-204.6</v>
+        <v>0</v>
       </c>
       <c r="AA22" s="3" t="s">
         <v>43</v>
@@ -4330,7 +4330,7 @@
         <v>43</v>
       </c>
       <c r="Z23" s="3">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="AA23" s="3" t="s">
         <v>43</v>
@@ -4461,7 +4461,7 @@
         <v>43</v>
       </c>
       <c r="Z24" s="3">
-        <v>-204.6</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="3" t="s">
         <v>43</v>
@@ -4592,7 +4592,7 @@
         <v>43</v>
       </c>
       <c r="Z25" s="3">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="AA25" s="3" t="s">
         <v>43</v>
@@ -12321,7 +12321,7 @@
         <v>43</v>
       </c>
       <c r="Z84" s="3">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="AA84" s="3" t="s">
         <v>43</v>
@@ -12452,7 +12452,7 @@
         <v>43</v>
       </c>
       <c r="Z85" s="3">
-        <v>-204.6</v>
+        <v>0</v>
       </c>
       <c r="AA85" s="3" t="s">
         <v>43</v>
@@ -12583,7 +12583,7 @@
         <v>43</v>
       </c>
       <c r="Z86" s="3">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="AA86" s="3" t="s">
         <v>43</v>
@@ -12714,7 +12714,7 @@
         <v>43</v>
       </c>
       <c r="Z87" s="3">
-        <v>-204.6</v>
+        <v>0</v>
       </c>
       <c r="AA87" s="3" t="s">
         <v>43</v>
@@ -14548,7 +14548,7 @@
         <v>43</v>
       </c>
       <c r="Z101" s="3">
-        <v>-64</v>
+        <v>0</v>
       </c>
       <c r="AA101" s="3" t="s">
         <v>43</v>
@@ -14810,7 +14810,7 @@
         <v>43</v>
       </c>
       <c r="Z103" s="3">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="AA103" s="3" t="s">
         <v>43</v>
@@ -14941,7 +14941,7 @@
         <v>43</v>
       </c>
       <c r="Z104" s="3">
-        <v>-128</v>
+        <v>0</v>
       </c>
       <c r="AA104" s="3" t="s">
         <v>43</v>
@@ -15072,7 +15072,7 @@
         <v>43</v>
       </c>
       <c r="Z105" s="3">
-        <v>-204.6</v>
+        <v>0</v>
       </c>
       <c r="AA105" s="3" t="s">
         <v>43</v>
@@ -15989,7 +15989,7 @@
         <v>43</v>
       </c>
       <c r="Z112" s="3">
-        <v>-64</v>
+        <v>0</v>
       </c>
       <c r="AA112" s="3" t="s">
         <v>43</v>
@@ -16251,7 +16251,7 @@
         <v>43</v>
       </c>
       <c r="Z114" s="3">
-        <v>-500</v>
+        <v>0</v>
       </c>
       <c r="AA114" s="3" t="s">
         <v>43</v>
@@ -16513,7 +16513,7 @@
         <v>43</v>
       </c>
       <c r="Z116" s="3">
-        <v>-128</v>
+        <v>0</v>
       </c>
       <c r="AA116" s="3" t="s">
         <v>43</v>
@@ -16644,7 +16644,7 @@
         <v>43</v>
       </c>
       <c r="Z117" s="3">
-        <v>-102.3</v>
+        <v>0</v>
       </c>
       <c r="AA117" s="3" t="s">
         <v>43</v>

</xml_diff>